<commit_message>
Fixed the Chrome and Firefox Issues
</commit_message>
<xml_diff>
--- a/src/main/java/com/hybridFramework/data/TestData.xlsx
+++ b/src/main/java/com/hybridFramework/data/TestData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>userName</t>
   </si>
@@ -34,6 +34,15 @@
   </si>
   <si>
     <t>y</t>
+  </si>
+  <si>
+    <t>testCaseName</t>
+  </si>
+  <si>
+    <t>TC_001</t>
+  </si>
+  <si>
+    <t>TC_002</t>
   </si>
 </sst>
 </file>
@@ -404,56 +413,67 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>